<commit_message>
added week 1 day 1 booth
</commit_message>
<xml_diff>
--- a/02-Lesson-Plans/01-Excel/1/Activities/05-Ins_Lookups/Solved/Lookups.xlsx
+++ b/02-Lesson-Plans/01-Excel/1/Activities/05-Ins_Lookups/Solved/Lookups.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomberton/Desktop/DV-Lesson-Plans/01-Excel/2/Activities/11-Ins_Lookups/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abooth\source\smu_new\UofM-VIRT-DATA-PT-03-2022-U-B\02-Lesson-Plans\01-Excel\1\Activities\05-Ins_Lookups\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454FF0F3-FCB9-AD45-AF4C-F7339BE56D07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16300" tabRatio="706" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="456" windowWidth="28044" windowHeight="12132" tabRatio="706"/>
   </bookViews>
   <sheets>
     <sheet name="VLookup" sheetId="1" r:id="rId1"/>
     <sheet name="HLookup" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Computer</t>
   </si>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +225,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{18E8DCA2-9109-4D20-8E7D-710CB276123C}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -538,32 +537,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="7" width="9.6640625" customWidth="1"/>
     <col min="8" max="9" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>104</v>
       </c>
@@ -571,8 +573,12 @@
         <f>VLOOKUP(A2,$E$4:$G$7,3,FALSE)</f>
         <v>Printer</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" t="str">
+        <f>VLOOKUP(A2,$E$3:$G$7,2, FALSE)</f>
+        <v>HP</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>103</v>
       </c>
@@ -580,6 +586,10 @@
         <f t="shared" ref="B3:B11" si="0">VLOOKUP(A3,$E$4:$G$7,3,FALSE)</f>
         <v>Mouse</v>
       </c>
+      <c r="C3" s="8" t="str">
+        <f t="shared" ref="C3:C11" si="1">VLOOKUP(A3,$E$3:$G$7,2, FALSE)</f>
+        <v>Logitech</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
@@ -590,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>104</v>
       </c>
@@ -598,6 +608,10 @@
         <f t="shared" si="0"/>
         <v>Printer</v>
       </c>
+      <c r="C4" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>HP</v>
+      </c>
       <c r="E4">
         <v>101</v>
       </c>
@@ -608,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>101</v>
       </c>
@@ -616,6 +630,10 @@
         <f t="shared" si="0"/>
         <v>Computer</v>
       </c>
+      <c r="C5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Dell</v>
+      </c>
       <c r="E5">
         <v>102</v>
       </c>
@@ -626,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>102</v>
       </c>
@@ -634,6 +652,10 @@
         <f t="shared" si="0"/>
         <v>Keyboard</v>
       </c>
+      <c r="C6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Logitech</v>
+      </c>
       <c r="E6">
         <v>103</v>
       </c>
@@ -644,7 +666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>103</v>
       </c>
@@ -652,6 +674,10 @@
         <f t="shared" si="0"/>
         <v>Mouse</v>
       </c>
+      <c r="C7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Logitech</v>
+      </c>
       <c r="E7">
         <v>104</v>
       </c>
@@ -662,7 +688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>101</v>
       </c>
@@ -670,8 +696,12 @@
         <f t="shared" si="0"/>
         <v>Computer</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Dell</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>104</v>
       </c>
@@ -679,8 +709,12 @@
         <f t="shared" si="0"/>
         <v>Printer</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>HP</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>101</v>
       </c>
@@ -688,14 +722,22 @@
         <f t="shared" si="0"/>
         <v>Computer</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Dell</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>102</v>
       </c>
       <c r="B11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Keyboard</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Logitech</v>
       </c>
     </row>
   </sheetData>
@@ -705,24 +747,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="7" width="9.6640625" customWidth="1"/>
     <col min="8" max="9" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -732,7 +774,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>104</v>
       </c>
@@ -741,7 +783,7 @@
         <v>Printer</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>103</v>
       </c>
@@ -750,7 +792,7 @@
         <v>Mouse</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>104</v>
       </c>
@@ -774,7 +816,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>101</v>
       </c>
@@ -798,7 +840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>102</v>
       </c>
@@ -822,7 +864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>103</v>
       </c>
@@ -831,7 +873,7 @@
         <v>Mouse</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>101</v>
       </c>
@@ -840,7 +882,7 @@
         <v>Computer</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>104</v>
       </c>
@@ -849,7 +891,7 @@
         <v>Printer</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>101</v>
       </c>
@@ -858,7 +900,7 @@
         <v>Computer</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>102</v>
       </c>

</xml_diff>